<commit_message>
added some imbie2 estimates
</commit_message>
<xml_diff>
--- a/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
+++ b/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag\Documents\Python\project01\data\raw_data\ComparisonEstimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D86B0B-BB02-4FC1-B36B-2ED22F47798E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC994CD1-1AF7-40D7-A037-DCB43AF7A131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GMSL" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="GrIS" sheetId="5" r:id="rId5"/>
     <sheet name="WAIS" sheetId="6" r:id="rId6"/>
     <sheet name="EAIS" sheetId="7" r:id="rId7"/>
-    <sheet name="Expert" sheetId="8" r:id="rId8"/>
+    <sheet name="Pen" sheetId="9" r:id="rId8"/>
+    <sheet name="Expert" sheetId="8" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="46">
   <si>
     <t>#</t>
   </si>
@@ -173,6 +174,9 @@
   </si>
   <si>
     <t xml:space="preserve">Table2 https://www.pnas.org/content/116/23/11195 </t>
+  </si>
+  <si>
+    <t>IMBIE 2, https://www.nature.com/articles/s41586-018-0179-y</t>
   </si>
 </sst>
 </file>
@@ -182,7 +186,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -239,6 +243,23 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF222222"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -273,7 +294,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -289,11 +310,13 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -517,7 +540,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -612,7 +635,7 @@
       <c r="E6" s="6">
         <v>0.03</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -637,7 +660,7 @@
       <c r="F7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>29</v>
       </c>
     </row>
@@ -737,7 +760,7 @@
       <c r="F5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>30</v>
       </c>
     </row>
@@ -763,24 +786,24 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>1850</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>1900</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <f t="shared" ref="D7:E7" si="0">0.014*100/50</f>
         <v>2.8000000000000004E-2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <f t="shared" si="0"/>
         <v>2.8000000000000004E-2</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="1" t="s">
@@ -904,30 +927,30 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>1850</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>1900</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="14">
         <f t="shared" ref="D7:E7" si="0">0.014*100/50</f>
         <v>2.8000000000000004E-2</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="14">
         <f t="shared" si="0"/>
         <v>2.8000000000000004E-2</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="14" t="s">
         <v>43</v>
       </c>
     </row>
@@ -944,10 +967,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G2"/>
+      <selection sqref="A1:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1002,50 +1025,59 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
+    <row r="5" spans="1:7" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="1">
-        <v>1993</v>
+        <v>1992</v>
       </c>
       <c r="C5" s="1">
         <v>2017</v>
       </c>
       <c r="D5" s="10">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="E5" s="11">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+        <f>0.0076/(C5-B5)</f>
+        <v>3.0400000000000002E-4</v>
+      </c>
+      <c r="E5" s="10">
+        <f>0.0039/(C5-B5)</f>
+        <v>1.56E-4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>1850</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>1900</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="14">
         <f t="shared" ref="D6:E6" si="0">0.014*100/50</f>
         <v>2.8000000000000004E-2</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="14">
         <f t="shared" si="0"/>
         <v>2.8000000000000004E-2</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="14" t="s">
         <v>20</v>
       </c>
+    </row>
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1057,7 +1089,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1125,7 +1157,7 @@
       <c r="C5" s="1">
         <v>2015</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <f>0.077-0.01</f>
         <v>6.7000000000000004E-2</v>
       </c>
@@ -1184,30 +1216,30 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>1850</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>1900</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="14">
         <f t="shared" ref="D8:E8" si="0">0.014*100/50</f>
         <v>2.8000000000000004E-2</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="14">
         <f t="shared" si="0"/>
         <v>2.8000000000000004E-2</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="15"/>
+      <c r="H8" s="14"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1222,12 +1254,96 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="2">
+        <v>0.95416999999999996</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1.6449</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1992</v>
+      </c>
+      <c r="C5" s="7">
+        <v>2017</v>
+      </c>
+      <c r="D5" s="17">
+        <f>94/361000</f>
+        <v>2.6038781163434903E-4</v>
+      </c>
+      <c r="E5" s="17">
+        <f>27/361000</f>
+        <v>7.4792243767313015E-5</v>
+      </c>
+      <c r="F5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="14"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="14"/>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1248,10 +1364,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E700963A-2E81-4D98-8532-52392815F16C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA05C6A7-BA3D-4777-877F-5B2D19C566E2}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1263,67 +1391,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="14" t="s">
+      <c r="A1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="14"/>
+      <c r="C1" s="13"/>
       <c r="E1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14" t="s">
+      <c r="A2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="14"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="14"/>
+      <c r="A3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D4" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E4" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G4" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="14">
+      <c r="B5" s="13">
         <v>2</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="13">
         <f>(0.7+1.5+1.5+2)/4</f>
         <v>1.425</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="13">
         <v>0.36</v>
       </c>
       <c r="E5">
@@ -1340,7 +1468,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="13" t="s">
         <v>32</v>
       </c>
       <c r="B6">
@@ -1367,13 +1495,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="14">
+      <c r="B7" s="13">
         <v>2</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="13">
         <f>(0.7+1.5+1.5+2)/4</f>
         <v>1.425</v>
       </c>
@@ -1394,7 +1522,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="13" t="s">
         <v>41</v>
       </c>
       <c r="B8">
@@ -1421,13 +1549,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="14">
+      <c r="B9" s="13">
         <v>2</v>
       </c>
-      <c r="C9" s="14">
+      <c r="C9" s="13">
         <f>(0.7+1.5+1.5+2)/4</f>
         <v>1.425</v>
       </c>
@@ -1448,7 +1576,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="13" t="s">
         <v>42</v>
       </c>
       <c r="B10">

</xml_diff>

<commit_message>
added tsls bar plot
</commit_message>
<xml_diff>
--- a/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
+++ b/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag\Documents\Python\project01\data\raw_data\ComparisonEstimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AEA2BED-8E2F-4325-B848-A28EDF64A899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76C90560-9A49-40AE-AFFC-CA34DE2C206D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GMSL" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="64">
   <si>
     <t>#</t>
   </si>
@@ -153,21 +153,9 @@
     <t>https://www.nature.com/articles/s41586-019-1071-0?TB_iframe=true&amp;width=921.6&amp;height=921.6</t>
   </si>
   <si>
-    <t>20c</t>
-  </si>
-  <si>
     <t>ar6 table 9.5</t>
   </si>
   <si>
-    <t>not really wais, ais</t>
-  </si>
-  <si>
-    <t>not really eais, ais</t>
-  </si>
-  <si>
-    <t>not really pen but, ais</t>
-  </si>
-  <si>
     <t>Thermal expansion</t>
   </si>
   <si>
@@ -241,16 +229,16 @@
   </si>
   <si>
     <t>ar6</t>
+  </si>
+  <si>
+    <t>Does this include the periphery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
-  </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -297,13 +285,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
@@ -345,7 +326,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -358,11 +339,6 @@
         <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -373,12 +349,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -386,28 +361,26 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -421,12 +394,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+  <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -679,7 +651,7 @@
       <c r="G2" s="2">
         <v>3.2896999999999998</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -687,13 +659,13 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="23"/>
-      <c r="P3" s="23"/>
-      <c r="Q3" s="23"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
     </row>
     <row r="4" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -717,17 +689,17 @@
       <c r="G4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
-      <c r="O4" s="23"/>
-      <c r="P4" s="23"/>
-      <c r="Q4" s="23"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
     </row>
     <row r="5" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" s="1">
         <v>1901</v>
@@ -735,26 +707,26 @@
       <c r="C5" s="1">
         <v>1990</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="21">
         <v>1.35</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="21">
         <v>0.34653615831230811</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
+      <c r="F5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
     </row>
     <row r="6" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1">
         <v>1971</v>
@@ -762,58 +734,58 @@
       <c r="C6" s="1">
         <v>2018</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="21">
         <v>2.33</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="21">
         <v>0.47724716539502088</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
+      <c r="F6" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
     </row>
     <row r="7" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="6">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5">
         <v>1993</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>2018</v>
       </c>
-      <c r="D7" s="18">
+      <c r="D7" s="16">
         <v>3.25</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="16">
         <v>0.22190473295437274</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
+      <c r="F7" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
     </row>
     <row r="8" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="6">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5">
         <v>2006</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>2018</v>
       </c>
       <c r="D8">
@@ -822,25 +794,25 @@
       <c r="E8">
         <v>0.29181992278931213</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
+      <c r="F8" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
     </row>
     <row r="9" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="6">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5">
         <v>1901</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>2018</v>
       </c>
       <c r="D9">
@@ -849,16 +821,16 @@
       <c r="E9">
         <v>0.27054138675259143</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
+      <c r="F9" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
     </row>
     <row r="10" spans="1:17" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -870,105 +842,105 @@
       <c r="C10" s="1">
         <v>1900</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <f>0.014*1000/50</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <f>0.014*1000/50</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
     </row>
     <row r="11" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
     </row>
     <row r="12" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
     </row>
     <row r="13" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K13" s="23"/>
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
     </row>
     <row r="14" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
     </row>
     <row r="15" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K15" s="23"/>
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
     </row>
     <row r="16" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K16" s="23"/>
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
     </row>
     <row r="17" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K17" s="23"/>
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
     </row>
     <row r="18" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q18" s="23"/>
+      <c r="Q18" s="21"/>
     </row>
     <row r="19" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q19" s="23"/>
+      <c r="Q19" s="21"/>
     </row>
     <row r="20" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q20" s="23"/>
+      <c r="Q20" s="21"/>
     </row>
     <row r="21" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q21" s="23"/>
+      <c r="Q21" s="21"/>
     </row>
     <row r="22" spans="11:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Q22" s="18"/>
+      <c r="Q22" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -990,431 +962,431 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="7.85546875" style="16" customWidth="1"/>
-    <col min="5" max="9" width="7.85546875" style="18" customWidth="1"/>
-    <col min="10" max="19" width="7.85546875" style="16" customWidth="1"/>
-    <col min="20" max="16384" width="9.140625" style="16"/>
+    <col min="1" max="4" width="7.85546875" style="14" customWidth="1"/>
+    <col min="5" max="9" width="7.85546875" style="16" customWidth="1"/>
+    <col min="10" max="19" width="7.85546875" style="14" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" s="26" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:18" s="24" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="I1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="K1" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25" t="s">
+      <c r="L1" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="M1" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G1" s="25" t="s">
+      <c r="N1" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="I1" s="25" t="s">
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="J1" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="K1" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="L1" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="N1" s="25" t="s">
-        <v>58</v>
-      </c>
-      <c r="O1" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="R1" s="25"/>
+      <c r="R1" s="23"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A2" s="23"/>
+      <c r="A2" s="21"/>
       <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="I2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="K2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="M2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="O2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q2" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="23" t="s">
-        <v>43</v>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="R2" s="21" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A3" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" s="6">
+      <c r="A3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="5">
         <v>1901</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>1990</v>
       </c>
-      <c r="D3" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="23">
+      <c r="D3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="21">
         <v>0.36</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="21">
         <f>ABS(0.17-0.54)/$B$19</f>
         <v>0.11247226190838071</v>
       </c>
-      <c r="G3" s="23">
+      <c r="G3" s="21">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H3" s="23">
+      <c r="H3" s="21">
         <f>ABS(0.34-0.82)/$B$19</f>
         <v>0.14590996139465603</v>
       </c>
-      <c r="I3" s="23">
+      <c r="I3" s="21">
         <v>0.33</v>
       </c>
-      <c r="J3" s="23">
+      <c r="J3" s="21">
         <f>ABS(0.18-0.47)/$B$19</f>
         <v>8.8153935009271364E-2</v>
       </c>
-      <c r="K3" s="23">
+      <c r="K3" s="21">
         <v>0</v>
       </c>
-      <c r="L3" s="23">
+      <c r="L3" s="21">
         <f>ABS(-0.1-0.11)/$B$19</f>
         <v>6.3835608110162034E-2</v>
       </c>
-      <c r="M3" s="23">
+      <c r="M3" s="21">
         <v>-0.15</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="21">
         <f>ABS(-0.35-0.04)/$B$19</f>
         <v>0.11855184363315803</v>
       </c>
-      <c r="O3" s="23">
+      <c r="O3" s="21">
         <v>1.1100000000000001</v>
       </c>
-      <c r="P3" s="23">
+      <c r="P3" s="21">
         <f>ABS(0.71-1.52)/$B$19</f>
         <v>0.24622305985348211</v>
       </c>
-      <c r="Q3" s="23">
+      <c r="Q3" s="21">
         <v>1.35</v>
       </c>
-      <c r="R3" s="23">
+      <c r="R3" s="21">
         <f>ABS(0.78-1.92)/$B$19</f>
         <v>0.34653615831230811</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A4" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="6">
+      <c r="A4" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="5">
         <v>1971</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>2018</v>
       </c>
-      <c r="D4" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="23">
+      <c r="D4" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="21">
         <v>1.01</v>
       </c>
-      <c r="F4" s="24">
+      <c r="F4" s="22">
         <f>ABS(0.73-1.29)/$B$19</f>
         <v>0.17022828829376541</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="21">
         <v>0.44</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="21">
         <f>ABS(0.21-0.67)/$B$19</f>
         <v>0.13983037966987874</v>
       </c>
-      <c r="I4" s="23">
+      <c r="I4" s="21">
         <v>0.25</v>
       </c>
-      <c r="J4" s="23">
+      <c r="J4" s="21">
         <f>ABS(0.16-0.34)/$B$19</f>
         <v>5.4716235522996023E-2</v>
       </c>
-      <c r="K4" s="23">
+      <c r="K4" s="21">
         <v>0.14000000000000001</v>
       </c>
-      <c r="L4" s="23">
+      <c r="L4" s="21">
         <f>ABS(-0.09-0.37)/$B$19</f>
         <v>0.13983037966987871</v>
       </c>
-      <c r="M4" s="23">
+      <c r="M4" s="21">
         <v>0.15</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="21">
         <f>ABS(-0.05-0.36)/$B$19</f>
         <v>0.12463142535793537</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="21">
         <v>2</v>
       </c>
-      <c r="P4" s="23">
+      <c r="P4" s="21">
         <f>ABS(1.52-2.49)/$B$19</f>
         <v>0.29485971365170083</v>
       </c>
-      <c r="Q4" s="23">
+      <c r="Q4" s="21">
         <v>2.33</v>
       </c>
-      <c r="R4" s="23">
+      <c r="R4" s="21">
         <f>ABS(1.55-3.12)/$B$19</f>
         <v>0.47724716539502088</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="5">
         <v>1993</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2018</v>
       </c>
-      <c r="D5" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E5" s="23">
+      <c r="D5" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="21">
         <v>1.31</v>
       </c>
-      <c r="F5" s="24">
+      <c r="F5" s="22">
         <f>ABS(0.95-1.66)/$B$19</f>
         <v>0.21582515122959539</v>
       </c>
-      <c r="G5" s="23">
+      <c r="G5" s="21">
         <v>0.55000000000000004</v>
       </c>
-      <c r="H5" s="23">
+      <c r="H5" s="21">
         <f>ABS(0.4-0.7)/$B$19</f>
         <v>9.1193725871660011E-2</v>
       </c>
-      <c r="I5" s="23">
+      <c r="I5" s="21">
         <v>0.43</v>
       </c>
-      <c r="J5" s="23">
+      <c r="J5" s="21">
         <f>ABS(0.36-0.51)/$B$19</f>
         <v>4.5596862935830026E-2</v>
       </c>
-      <c r="K5" s="23">
+      <c r="K5" s="21">
         <v>0.25</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="21">
         <f>ABS(0.16-0.33)/$B$19</f>
         <v>5.1676444660607355E-2</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M5" s="21">
         <v>0.31</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="21">
         <f>ABS(0.13-0.49)/$B$19</f>
         <v>0.10943247104599203</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="21">
         <v>2.85</v>
       </c>
-      <c r="P5" s="23">
+      <c r="P5" s="21">
         <f>ABS(2.41-3.29)/$B$19</f>
         <v>0.26750159589020273</v>
       </c>
-      <c r="Q5" s="23">
+      <c r="Q5" s="21">
         <v>3.25</v>
       </c>
-      <c r="R5" s="23">
+      <c r="R5" s="21">
         <f>ABS(2.88-3.61)/$B$19</f>
         <v>0.22190473295437274</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="5">
         <v>2006</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>2018</v>
       </c>
-      <c r="D6" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="23">
+      <c r="D6" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="21">
         <v>1.39</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="21">
         <f>ABS(0.74-2.05)/$B$19</f>
         <v>0.39821260297291544</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="21">
         <v>0.62</v>
       </c>
-      <c r="H6" s="23">
+      <c r="H6" s="21">
         <f>ABS(0.57-0.68)/$B$19</f>
         <v>3.3437699486275375E-2</v>
       </c>
-      <c r="I6" s="23">
+      <c r="I6" s="21">
         <v>0.63</v>
       </c>
-      <c r="J6" s="23">
+      <c r="J6" s="21">
         <f>ABS(0.51-0.74)/$B$19</f>
         <v>6.9915189834939356E-2</v>
       </c>
-      <c r="K6" s="23">
+      <c r="K6" s="21">
         <v>0.37</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="21">
         <f>ABS(0.24-0.5)/$B$19</f>
         <v>7.9034562422105367E-2</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="21">
         <v>0.6</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="21">
         <f>ABS(0.32-0.88)/$B$19</f>
         <v>0.17022828829376541</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="21">
         <v>3.61</v>
       </c>
-      <c r="P6" s="23">
+      <c r="P6" s="21">
         <f>ABS(2.88-4.35)/$B$19</f>
         <v>0.44684925677113407</v>
       </c>
-      <c r="Q6" s="23">
+      <c r="Q6" s="21">
         <v>3.69</v>
       </c>
-      <c r="R6" s="23">
+      <c r="R6" s="21">
         <f>ABS(3.21-4.17)/$B$19</f>
         <v>0.29181992278931213</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="A7" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="5">
         <v>1901</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>2018</v>
       </c>
-      <c r="D7" s="23" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="23">
+      <c r="D7" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="21">
         <v>0.54</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="21">
         <f>ABS(0.4 -0.68)/$B$19</f>
         <v>8.5114144146882703E-2</v>
       </c>
-      <c r="G7" s="23">
+      <c r="G7" s="21">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H7" s="23">
+      <c r="H7" s="21">
         <f>ABS(0.36-0.79)/$B$19</f>
         <v>0.13071100708271274</v>
       </c>
-      <c r="I7" s="23">
+      <c r="I7" s="21">
         <v>0.35</v>
       </c>
-      <c r="J7" s="23">
+      <c r="J7" s="21">
         <f>ABS(0.23-0.46)/$B$19</f>
         <v>6.9915189834939356E-2</v>
       </c>
-      <c r="K7" s="23">
+      <c r="K7" s="21">
         <v>0.06</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="21">
         <f>ABS(-0.03-0.15)/$B$19</f>
         <v>5.4716235522996017E-2</v>
       </c>
-      <c r="M7" s="23">
+      <c r="M7" s="21">
         <v>-0.11</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="21">
         <f>ABS(-0.39-0.17)/$B$19</f>
         <v>0.17022828829376541</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="21">
         <v>1.41</v>
       </c>
-      <c r="P7" s="23">
+      <c r="P7" s="21">
         <f>ABS(1-1.82)/$B$19</f>
         <v>0.24926285071587079</v>
       </c>
-      <c r="Q7" s="23">
+      <c r="Q7" s="21">
         <v>1.73</v>
       </c>
-      <c r="R7" s="23">
+      <c r="R7" s="21">
         <f>ABS(1.28-2.17)/$B$19</f>
         <v>0.27054138675259143</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
@@ -1424,17 +1396,17 @@
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
-      <c r="O8" s="23"/>
-      <c r="P8" s="23"/>
-      <c r="Q8" s="23"/>
-      <c r="R8" s="23"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
       <c r="D9"/>
       <c r="E9"/>
       <c r="F9"/>
@@ -1444,15 +1416,15 @@
       <c r="J9"/>
       <c r="K9"/>
       <c r="L9"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
@@ -1471,8 +1443,8 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
@@ -1490,62 +1462,62 @@
       <c r="R11"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A12" s="23"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="23"/>
-      <c r="D12" s="23"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A13" s="23"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A14" s="23"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="23"/>
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
+      <c r="A16" s="21"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="21"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B19" s="2">
@@ -1553,20 +1525,20 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="16" t="s">
-        <v>63</v>
+      <c r="A21" s="14" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="16" t="s">
-        <v>61</v>
+      <c r="A22" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="E23" s="20"/>
+      <c r="E23" s="18"/>
     </row>
     <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.2">
-      <c r="E24" s="20"/>
+      <c r="E24" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1610,7 +1582,7 @@
       <c r="G2" s="2">
         <v>3.2896999999999998</v>
       </c>
-      <c r="H2" s="14"/>
+      <c r="H2" s="12"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1639,17 +1611,17 @@
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K4" s="15"/>
-      <c r="L4" s="15"/>
-      <c r="M4" s="17"/>
-      <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
+      <c r="K4" s="13"/>
+      <c r="L4" s="13"/>
+      <c r="M4" s="15"/>
+      <c r="N4" s="15"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>1901</v>
@@ -1664,20 +1636,20 @@
         <v>0.11247226190838071</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G5" s="9"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="17"/>
-      <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
+        <v>37</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="K5" s="13"/>
+      <c r="L5" s="13"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>1971</v>
@@ -1691,20 +1663,20 @@
       <c r="E6">
         <v>0.17022828829376541</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-    </row>
-    <row r="7" spans="1:17" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+    </row>
+    <row r="7" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>1993</v>
@@ -1718,16 +1690,16 @@
       <c r="E7">
         <v>0.21582515122959539</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>62</v>
+      <c r="F7" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="19" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>2006</v>
@@ -1744,7 +1716,7 @@
     </row>
     <row r="9" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>1901</v>
@@ -1771,7 +1743,7 @@
   </sheetPr>
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -1787,7 +1759,7 @@
       <c r="G1" s="2">
         <v>0.95416999999999996</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1804,7 +1776,7 @@
       <c r="G2" s="2">
         <v>3.2896999999999998</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1812,8 +1784,8 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="21" t="s">
-        <v>38</v>
+      <c r="I3" s="19" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
@@ -1838,22 +1810,22 @@
       <c r="G4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="N4" s="15"/>
-      <c r="O4" s="17"/>
-      <c r="P4" s="17"/>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="17"/>
-      <c r="S4" s="17"/>
+      <c r="M4" s="13"/>
+      <c r="N4" s="13"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="15"/>
+      <c r="S4" s="15"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="6">
+      <c r="A5" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5">
         <v>1901</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>1990</v>
       </c>
       <c r="D5">
@@ -1862,26 +1834,26 @@
       <c r="E5">
         <v>0.14590996139465603</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>66</v>
+      <c r="F5" s="12" t="s">
+        <v>62</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="M5" s="15"/>
-      <c r="N5" s="15"/>
-      <c r="O5" s="17"/>
-      <c r="P5" s="17"/>
-      <c r="Q5" s="17"/>
-      <c r="R5" s="17"/>
-      <c r="S5" s="17"/>
+      <c r="M5" s="13"/>
+      <c r="N5" s="13"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A6" s="23" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="6">
+      <c r="A6" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5">
         <v>1971</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>2018</v>
       </c>
       <c r="D6">
@@ -1890,25 +1862,25 @@
       <c r="E6">
         <v>0.13983037966987874</v>
       </c>
-      <c r="F6" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="M6" s="16"/>
-      <c r="N6" s="16"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-    </row>
-    <row r="7" spans="1:19" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="23" t="s">
-        <v>49</v>
-      </c>
-      <c r="B7" s="6">
+      <c r="F6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+    </row>
+    <row r="7" spans="1:19" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="5">
         <v>1993</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>2018</v>
       </c>
       <c r="D7">
@@ -1917,19 +1889,19 @@
       <c r="E7">
         <v>9.1193725871660011E-2</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="G7" s="22"/>
+      <c r="F7" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="G7" s="20"/>
     </row>
     <row r="8" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="6">
+      <c r="A8" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="5">
         <v>2006</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>2018</v>
       </c>
       <c r="D8">
@@ -1938,25 +1910,25 @@
       <c r="E8">
         <v>3.3437699486275375E-2</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="M8" s="16"/>
-      <c r="N8" s="16"/>
-      <c r="O8" s="19"/>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="18"/>
-      <c r="S8" s="18"/>
+      <c r="F8" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="23" t="s">
-        <v>52</v>
-      </c>
-      <c r="B9" s="6">
+      <c r="A9" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5">
         <v>1901</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>2018</v>
       </c>
       <c r="D9">
@@ -1965,52 +1937,52 @@
       <c r="E9">
         <v>0.13071100708271274</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="M9" s="16"/>
-      <c r="N9" s="16"/>
-      <c r="O9" s="18"/>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="18"/>
-      <c r="S9" s="18"/>
+      <c r="F9" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="16"/>
+      <c r="P9" s="16"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
     </row>
     <row r="10" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M10" s="16"/>
-      <c r="N10" s="16"/>
-      <c r="O10" s="18"/>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="18"/>
-      <c r="S10" s="18"/>
+      <c r="M10" s="14"/>
+      <c r="N10" s="14"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
+      <c r="R10" s="16"/>
+      <c r="S10" s="16"/>
     </row>
     <row r="11" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M11" s="16"/>
-      <c r="N11" s="16"/>
-      <c r="O11" s="18"/>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="18"/>
-      <c r="S11" s="18"/>
+      <c r="M11" s="14"/>
+      <c r="N11" s="14"/>
+      <c r="O11" s="16"/>
+      <c r="P11" s="16"/>
+      <c r="Q11" s="16"/>
+      <c r="R11" s="16"/>
+      <c r="S11" s="16"/>
     </row>
     <row r="12" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M12" s="16"/>
-      <c r="N12" s="16"/>
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
+      <c r="M12" s="14"/>
+      <c r="N12" s="14"/>
+      <c r="O12" s="16"/>
+      <c r="P12" s="16"/>
+      <c r="Q12" s="16"/>
+      <c r="R12" s="16"/>
+      <c r="S12" s="16"/>
     </row>
     <row r="13" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="18"/>
-      <c r="P13" s="18"/>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="18"/>
-      <c r="S13" s="18"/>
+      <c r="M13" s="14"/>
+      <c r="N13" s="14"/>
+      <c r="O13" s="16"/>
+      <c r="P13" s="16"/>
+      <c r="Q13" s="16"/>
+      <c r="R13" s="16"/>
+      <c r="S13" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2028,7 +2000,7 @@
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:R24"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2036,7 +2008,7 @@
     <col min="2" max="3" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2046,11 +2018,11 @@
       <c r="G1" s="2">
         <v>0.95416999999999996</v>
       </c>
-      <c r="I1" s="14" t="s">
+      <c r="I1" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -2061,15 +2033,23 @@
         <v>3.2896999999999998</v>
       </c>
       <c r="H2" s="1"/>
-      <c r="I2" s="7" t="s">
+      <c r="I2">
+        <f>75.1/361</f>
+        <v>0.20803324099722989</v>
+      </c>
+      <c r="J2" s="12">
+        <f>29.4/361</f>
+        <v>8.1440443213296396E-2</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="1"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="L2" s="19" t="s">
+        <v>63</v>
+      </c>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -2099,7 +2079,7 @@
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5">
         <v>1901</v>
@@ -2114,20 +2094,20 @@
         <v>8.8153935009271364E-2</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="G5" s="1"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B6">
         <v>1971</v>
@@ -2141,20 +2121,20 @@
       <c r="E6">
         <v>5.4716235522996023E-2</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
+      <c r="F6" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>1993</v>
@@ -2168,25 +2148,25 @@
       <c r="E7">
         <v>4.5596862935830026E-2</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-    </row>
-    <row r="8" spans="1:18" s="21" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="B8" s="21">
+      <c r="F7" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+    </row>
+    <row r="8" spans="1:18" s="19" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="19">
         <v>2006</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="19">
         <v>2018</v>
       </c>
       <c r="D8">
@@ -2195,13 +2175,13 @@
       <c r="E8">
         <v>6.9915189834939356E-2</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>64</v>
+      <c r="F8" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>1901</v>
@@ -2215,92 +2195,93 @@
       <c r="E9">
         <v>6.9915189834939356E-2</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="23"/>
-      <c r="P9" s="23"/>
-      <c r="Q9" s="23"/>
-      <c r="R9" s="23"/>
+      <c r="F9" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
-      <c r="O10" s="23"/>
-      <c r="P10" s="23"/>
-      <c r="Q10" s="23"/>
-      <c r="R10" s="23"/>
+      <c r="A10" s="12"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="23"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="23"/>
-      <c r="R11" s="23"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="23"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="23"/>
-      <c r="R12" s="23"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
     </row>
     <row r="13" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L13" s="23"/>
-      <c r="M13" s="23"/>
-      <c r="N13" s="23"/>
-      <c r="O13" s="23"/>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="23"/>
-      <c r="R13" s="23"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
-      <c r="O14" s="23"/>
-      <c r="P14" s="23"/>
-      <c r="Q14" s="23"/>
-      <c r="R14" s="23"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L15" s="23"/>
-      <c r="M15" s="23"/>
-      <c r="N15" s="23"/>
-      <c r="O15" s="23"/>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="23"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L16" s="23"/>
-      <c r="M16" s="23"/>
-      <c r="N16" s="23"/>
-      <c r="O16" s="23"/>
-      <c r="P16" s="23"/>
-      <c r="Q16" s="23"/>
-      <c r="R16" s="23"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
     </row>
     <row r="17" spans="12:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="L17" s="23"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{37DEF5A8-E9F1-46C3-BAEE-FFDF254259B3}"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{37DEF5A8-E9F1-46C3-BAEE-FFDF254259B3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2340,7 +2321,7 @@
       <c r="G2" s="2">
         <v>3.2896999999999998</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="I2" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2348,7 +2329,7 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9"/>
+      <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -2373,49 +2354,49 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="21">
+    <row r="5" spans="1:13" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="19">
         <v>1901</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="19">
         <v>1990</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="19">
         <v>0</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="19">
         <v>6.3835608110162034E-2</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A6" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="21">
+      <c r="F5" s="19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="19" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="19">
         <v>1971</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="19">
         <v>2018</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="19">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="19">
         <v>0.13983037966987871</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>64</v>
+      <c r="F6" s="19" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B7">
         <v>1993</v>
@@ -2429,13 +2410,13 @@
       <c r="E7">
         <v>5.1676444660607355E-2</v>
       </c>
-      <c r="F7" s="14" t="s">
-        <v>64</v>
+      <c r="F7" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B8">
         <v>2006</v>
@@ -2449,13 +2430,13 @@
       <c r="E8">
         <v>7.9034562422105367E-2</v>
       </c>
-      <c r="F8" s="14" t="s">
-        <v>64</v>
+      <c r="F8" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>1901</v>
@@ -2469,93 +2450,93 @@
       <c r="E9">
         <v>5.4716235522996017E-2</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>64</v>
+      <c r="F9" s="12" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="11"/>
+      <c r="E10" s="9"/>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="M14" s="17"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
+      <c r="M14" s="15"/>
     </row>
     <row r="22" spans="7:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18"/>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
     </row>
     <row r="23" spans="7:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+      <c r="L23" s="16"/>
+      <c r="M23" s="16"/>
     </row>
     <row r="24" spans="7:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
+      <c r="G24" s="14"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="16"/>
     </row>
     <row r="25" spans="7:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G25" s="16"/>
-      <c r="H25" s="16"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="16"/>
+      <c r="K25" s="16"/>
+      <c r="L25" s="16"/>
+      <c r="M25" s="16"/>
     </row>
     <row r="26" spans="7:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G26" s="16"/>
-      <c r="H26" s="16"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="16"/>
+      <c r="K26" s="16"/>
+      <c r="L26" s="16"/>
+      <c r="M26" s="16"/>
     </row>
     <row r="27" spans="7:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G27" s="16"/>
-      <c r="H27" s="16"/>
-      <c r="I27" s="18"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="16"/>
+      <c r="K27" s="16"/>
+      <c r="L27" s="16"/>
+      <c r="M27" s="16"/>
     </row>
     <row r="28" spans="7:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="20"/>
-      <c r="J28" s="20"/>
-      <c r="K28" s="20"/>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
     </row>
     <row r="29" spans="7:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="20"/>
-      <c r="J29" s="20"/>
-      <c r="K29" s="20"/>
-      <c r="L29" s="20"/>
-      <c r="M29" s="20"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2568,45 +2549,45 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2">
         <v>0.95416999999999996</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="2">
         <v>3.2896999999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -2629,50 +2610,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1992</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2017</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="11">
         <f>94/3610</f>
         <v>2.6038781163434901E-2</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <f>27/3610</f>
         <v>7.479224376731302E-3</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="10">
-        <v>1901</v>
-      </c>
-      <c r="C6" s="10">
-        <v>1990</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>6.3835608110162034E-2</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -2685,19 +2642,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2">
@@ -2705,10 +2662,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="2">
@@ -2716,10 +2673,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2747,48 +2704,25 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1992</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2017</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="11">
         <f>-5/3610</f>
         <v>-1.3850415512465374E-3</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <f>46/3610</f>
         <v>1.2742382271468145E-2</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="10">
-        <v>1901</v>
-      </c>
-      <c r="C6" s="10">
-        <v>1990</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>6.3835608110162034E-2</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2798,19 +2732,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E700963A-2E81-4D98-8532-52392815F16C}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="2">
@@ -2818,10 +2752,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="2">
@@ -2829,10 +2763,10 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2860,48 +2794,25 @@
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>1992</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2017</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="11">
         <f>20/3610</f>
         <v>5.5401662049861496E-3</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="11">
         <f>15/3610</f>
         <v>4.1551246537396124E-3</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="10">
-        <v>1901</v>
-      </c>
-      <c r="C6" s="10">
-        <v>1990</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>6.3835608110162034E-2</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="G6" s="10" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2925,67 +2836,67 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="9"/>
+      <c r="C1" s="8"/>
       <c r="E1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="9" t="s">
+      <c r="H4" s="8" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="8">
         <v>2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="8">
         <f>(0.7+1.5+1.5+2)/4</f>
         <v>1.425</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="8">
         <v>0.36</v>
       </c>
       <c r="E5">
@@ -3002,7 +2913,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
       <c r="B6">
@@ -3029,13 +2940,13 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>2</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="8">
         <f>(0.7+1.5+1.5+2)/4</f>
         <v>1.425</v>
       </c>
@@ -3056,7 +2967,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
       <c r="B8">
@@ -3083,13 +2994,13 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>2</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="8">
         <f>(0.7+1.5+1.5+2)/4</f>
         <v>1.425</v>
       </c>
@@ -3110,7 +3021,7 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="8" t="s">
         <v>30</v>
       </c>
       <c r="B10">

</xml_diff>

<commit_message>
weighted regression and added experts
</commit_message>
<xml_diff>
--- a/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
+++ b/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uob-my.sharepoint.com/personal/ggjlb_bristol_ac_uk/Documents/docs/projects/CMIP6 Hackathon/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag\Documents\Python\project01\data\raw_data\ComparisonEstimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="13_ncr:1_{62BCE873-05FC-4628-B3F3-E0F4FE6B7E16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCF015DE-E9A2-4B60-B73B-9FDF77ECB046}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D2F90A5-CE20-4CC2-8F70-1462FEB0618C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28995" yWindow="16830" windowWidth="21525" windowHeight="14850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GMSL" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="68">
   <si>
     <t>#</t>
   </si>
@@ -232,6 +232,18 @@
   </si>
   <si>
     <t>Frederikse</t>
+  </si>
+  <si>
+    <t>FrederikseRate</t>
+  </si>
+  <si>
+    <t>#1901-2018</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -618,8 +630,8 @@
   </sheetPr>
   <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -681,7 +693,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -825,7 +837,7 @@
     </row>
     <row r="9" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B9" s="5">
         <v>1901</v>
@@ -1575,7 +1587,7 @@
   <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1625,7 +1637,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -1756,7 +1768,7 @@
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>1901</v>
@@ -1787,7 +1799,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1845,7 +1857,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -1983,8 +1995,8 @@
       <c r="T8" s="16"/>
     </row>
     <row r="9" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>47</v>
+      <c r="A9" t="s">
+        <v>65</v>
       </c>
       <c r="B9" s="5">
         <v>1901</v>
@@ -2064,7 +2076,7 @@
   <dimension ref="A1:S17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D4"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2132,7 +2144,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -2263,7 +2275,7 @@
     </row>
     <row r="9" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>1901</v>
@@ -2380,7 +2392,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2430,7 +2442,7 @@
         <v>5</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>6</v>
+        <v>64</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>6</v>
@@ -2539,7 +2551,7 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>47</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>1901</v>
@@ -2658,7 +2670,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2922,10 +2934,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA05C6A7-BA3D-4777-877F-5B2D19C566E2}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2935,7 +2947,7 @@
     <col min="4" max="9" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2947,7 +2959,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -2956,13 +2968,16 @@
       </c>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="B4" s="8" t="s">
         <v>22</v>
       </c>
@@ -2985,7 +3000,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>21</v>
       </c>
@@ -3012,7 +3027,7 @@
         <v>1.26</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>21</v>
       </c>
@@ -3039,7 +3054,7 @@
         <v>2.38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>29</v>
       </c>
@@ -3066,7 +3081,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="8" t="s">
         <v>29</v>
       </c>
@@ -3092,8 +3107,11 @@
       <c r="H8">
         <v>1.32</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
         <v>30</v>
       </c>
@@ -3120,7 +3138,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
comparisons and colors updated
</commit_message>
<xml_diff>
--- a/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
+++ b/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag\Documents\Python\project01\data\raw_data\ComparisonEstimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58CF08F2-9331-4995-BAD7-0B30A94B12F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF8D304-C2ED-4C2E-9B04-1B63CD2F0E0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GMSL" sheetId="1" r:id="rId1"/>
@@ -1650,8 +1650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1140D5A-6A3D-4D73-8C57-3CF86E2ECC01}">
   <dimension ref="A2:E168"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4967,8 +4967,8 @@
   </sheetPr>
   <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
all but glaciers added
</commit_message>
<xml_diff>
--- a/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
+++ b/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag\Documents\Python\project01\data\raw_data\ComparisonEstimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67159727-5128-4F20-A4E1-0A8384CC4AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7D5A70-A8BD-4E66-9C5D-B7B26F8D5786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GMSL" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="WAIS" sheetId="6" r:id="rId6"/>
     <sheet name="EAIS" sheetId="7" r:id="rId7"/>
     <sheet name="PEN" sheetId="9" r:id="rId8"/>
-    <sheet name="Expert" sheetId="8" r:id="rId9"/>
-    <sheet name="transposed ar6" sheetId="11" r:id="rId10"/>
-    <sheet name="Frederikse" sheetId="12" r:id="rId11"/>
+    <sheet name="AllButGlaciers" sheetId="13" r:id="rId9"/>
+    <sheet name="Expert" sheetId="8" r:id="rId10"/>
+    <sheet name="transposed ar6" sheetId="11" r:id="rId11"/>
+    <sheet name="Frederikse" sheetId="12" r:id="rId12"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="89">
   <si>
     <t>#</t>
   </si>
@@ -297,6 +297,18 @@
   </si>
   <si>
     <t>Directly from frederikse data file … 90% comnverted to sigma</t>
+  </si>
+  <si>
+    <t>glac</t>
+  </si>
+  <si>
+    <t>glacsigma</t>
+  </si>
+  <si>
+    <t>gmslrate</t>
+  </si>
+  <si>
+    <t>gmslsigma</t>
   </si>
 </sst>
 </file>
@@ -699,7 +711,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection sqref="A1:K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1055,6 +1067,244 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA05C6A7-BA3D-4777-877F-5B2D19C566E2}">
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="E1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="8"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="8">
+        <v>2</v>
+      </c>
+      <c r="C5" s="8">
+        <f>(0.7+1.5+1.5+2)/4</f>
+        <v>1.425</v>
+      </c>
+      <c r="D5" s="8">
+        <v>0.36</v>
+      </c>
+      <c r="E5">
+        <v>0.49</v>
+      </c>
+      <c r="F5">
+        <v>0.69</v>
+      </c>
+      <c r="G5">
+        <v>0.98</v>
+      </c>
+      <c r="H5">
+        <v>1.26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>(0.7+2+2+5)/4</f>
+        <v>2.4249999999999998</v>
+      </c>
+      <c r="D6">
+        <v>0.62</v>
+      </c>
+      <c r="E6">
+        <v>0.79</v>
+      </c>
+      <c r="F6">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G6">
+        <v>1.74</v>
+      </c>
+      <c r="H6">
+        <v>2.38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8">
+        <f>(0.7+1.5+1.5+2)/4</f>
+        <v>1.425</v>
+      </c>
+      <c r="D7">
+        <v>-0.08</v>
+      </c>
+      <c r="E7">
+        <v>-0.01</v>
+      </c>
+      <c r="F7">
+        <v>0.09</v>
+      </c>
+      <c r="G7">
+        <v>0.26</v>
+      </c>
+      <c r="H7">
+        <v>0.53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <f>(0.7+2+2+5)/4</f>
+        <v>2.4249999999999998</v>
+      </c>
+      <c r="D8">
+        <v>-0.11</v>
+      </c>
+      <c r="E8">
+        <v>0.02</v>
+      </c>
+      <c r="F8">
+        <v>0.21</v>
+      </c>
+      <c r="G8">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="H8">
+        <v>1.32</v>
+      </c>
+      <c r="I8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="8">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8">
+        <f>(0.7+1.5+1.5+2)/4</f>
+        <v>1.425</v>
+      </c>
+      <c r="D9">
+        <v>0.02</v>
+      </c>
+      <c r="E9">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.13</v>
+      </c>
+      <c r="G9">
+        <v>0.31</v>
+      </c>
+      <c r="H9">
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <f>(0.7+2+2+5)/4</f>
+        <v>2.4249999999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.02</v>
+      </c>
+      <c r="E10">
+        <v>0.1</v>
+      </c>
+      <c r="F10">
+        <v>0.23</v>
+      </c>
+      <c r="G10">
+        <v>0.6</v>
+      </c>
+      <c r="H10">
+        <v>0.99</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{031DC691-DD2C-453E-9956-962ECE938F19}">
   <dimension ref="A1:R24"/>
   <sheetViews>
@@ -1647,7 +1897,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1140D5A-6A3D-4D73-8C57-3CF86E2ECC01}">
   <dimension ref="A2:E168"/>
   <sheetViews>
@@ -4692,7 +4942,7 @@
   <dimension ref="A1:T13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="E5" sqref="E5:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5653,7 +5903,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -5826,239 +6076,303 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA05C6A7-BA3D-4777-877F-5B2D19C566E2}">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0414F62-F26B-4AD1-AB30-17B83DAD40A3}">
+  <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="11" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="E1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="D1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="2">
+        <v>0.95416999999999996</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="8"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="G2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" s="2">
+        <v>3.2896999999999998</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="8">
-        <v>2</v>
-      </c>
-      <c r="C5" s="8">
-        <f>(0.7+1.5+1.5+2)/4</f>
-        <v>1.425</v>
-      </c>
-      <c r="D5" s="8">
-        <v>0.36</v>
-      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="J4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" t="s">
+        <v>88</v>
+      </c>
+      <c r="L4" t="s">
+        <v>85</v>
+      </c>
+      <c r="M4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1901</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1990</v>
+      </c>
+      <c r="D5" s="5"/>
       <c r="E5">
-        <v>0.49</v>
+        <f>J5-L5</f>
+        <v>0.77000000000000013</v>
       </c>
       <c r="F5">
-        <v>0.69</v>
-      </c>
-      <c r="G5">
-        <v>0.98</v>
-      </c>
-      <c r="H5">
-        <v>1.26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6">
-        <f>(0.7+2+2+5)/4</f>
-        <v>2.4249999999999998</v>
-      </c>
-      <c r="D6">
+        <f>SQRT(K5^2+ M5^2)</f>
+        <v>0.37600136416247626</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J5" s="21">
+        <v>1.35</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0.34653615831230811</v>
+      </c>
+      <c r="L5">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="M5">
+        <v>0.14590996139465603</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="5">
+        <v>1971</v>
+      </c>
+      <c r="C6" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6">
+        <f>J6-L6</f>
+        <v>1.8900000000000001</v>
+      </c>
+      <c r="F6">
+        <f>SQRT(K6^2+ M6^2)</f>
+        <v>0.49731015669922207</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J6" s="21">
+        <v>2.33</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0.47724716539502088</v>
+      </c>
+      <c r="L6">
+        <v>0.44</v>
+      </c>
+      <c r="M6">
+        <v>0.13983037966987874</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1993</v>
+      </c>
+      <c r="C7" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7">
+        <f>J7-L7</f>
+        <v>2.7</v>
+      </c>
+      <c r="F7">
+        <f>SQRT(K7^2+ M7^2)</f>
+        <v>0.23991249685230437</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="16">
+        <v>3.25</v>
+      </c>
+      <c r="K7" s="16">
+        <v>0.22190473295437274</v>
+      </c>
+      <c r="L7">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M7">
+        <v>9.1193725871660011E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="5">
+        <v>2006</v>
+      </c>
+      <c r="C8" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8">
+        <f>J8-L8</f>
+        <v>3.07</v>
+      </c>
+      <c r="F8">
+        <f>SQRT(K8^2+ M8^2)</f>
+        <v>0.29372937729089094</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J8">
+        <v>3.69</v>
+      </c>
+      <c r="K8">
+        <v>0.29181992278931213</v>
+      </c>
+      <c r="L8">
         <v>0.62</v>
       </c>
-      <c r="E6">
-        <v>0.79</v>
-      </c>
-      <c r="F6">
-        <v>1.1100000000000001</v>
-      </c>
-      <c r="G6">
-        <v>1.74</v>
-      </c>
-      <c r="H6">
-        <v>2.38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="8">
-        <v>2</v>
-      </c>
-      <c r="C7" s="8">
-        <f>(0.7+1.5+1.5+2)/4</f>
-        <v>1.425</v>
-      </c>
-      <c r="D7">
-        <v>-0.08</v>
-      </c>
-      <c r="E7">
-        <v>-0.01</v>
-      </c>
-      <c r="F7">
-        <v>0.09</v>
-      </c>
-      <c r="G7">
-        <v>0.26</v>
-      </c>
-      <c r="H7">
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <f>(0.7+2+2+5)/4</f>
-        <v>2.4249999999999998</v>
-      </c>
-      <c r="D8">
-        <v>-0.11</v>
-      </c>
-      <c r="E8">
-        <v>0.02</v>
-      </c>
-      <c r="F8">
-        <v>0.21</v>
-      </c>
-      <c r="G8">
+      <c r="M8">
+        <v>3.3437699486275375E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1901</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9">
+        <f>J9-L9</f>
+        <v>1.1600000000000001</v>
+      </c>
+      <c r="F9">
+        <f>SQRT(K9^2+ M9^2)</f>
+        <v>0.30046299159562434</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9">
+        <v>1.73</v>
+      </c>
+      <c r="K9">
+        <v>0.27054138675259143</v>
+      </c>
+      <c r="L9">
         <v>0.56999999999999995</v>
       </c>
-      <c r="H8">
-        <v>1.32</v>
-      </c>
-      <c r="I8" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" s="8">
-        <v>2</v>
-      </c>
-      <c r="C9" s="8">
-        <f>(0.7+1.5+1.5+2)/4</f>
-        <v>1.425</v>
-      </c>
-      <c r="D9">
-        <v>0.02</v>
-      </c>
-      <c r="E9">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="F9">
-        <v>0.13</v>
-      </c>
-      <c r="G9">
-        <v>0.31</v>
-      </c>
-      <c r="H9">
-        <v>0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <f>(0.7+2+2+5)/4</f>
-        <v>2.4249999999999998</v>
-      </c>
-      <c r="D10">
-        <v>0.02</v>
-      </c>
+      <c r="M9">
+        <v>0.13071100708271274</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1850</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1900</v>
+      </c>
+      <c r="D10" s="5"/>
       <c r="E10">
-        <v>0.1</v>
+        <f>J10-L10</f>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F10">
-        <v>0.23</v>
-      </c>
-      <c r="G10">
-        <v>0.6</v>
-      </c>
-      <c r="H10">
-        <v>0.99</v>
+        <f>SQRT(K10^2+ M10^2)</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="5">
+        <f>0.014*1000/50</f>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="K10" s="5">
+        <f>0.014*1000/50</f>
+        <v>0.28000000000000003</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I1" r:id="rId1" xr:uid="{F141555B-26A2-40A5-8281-236CFCC5783A}"/>
+    <hyperlink ref="I2" r:id="rId2" xr:uid="{64358BC0-D5B0-428D-93C6-17383AB8397E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rename glaciers to GIC
</commit_message>
<xml_diff>
--- a/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
+++ b/data/raw_data/ComparisonEstimates/ComparisonSLRrates.xlsx
@@ -8,20 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ag\Documents\Python\project01\data\raw_data\ComparisonEstimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7D5A70-A8BD-4E66-9C5D-B7B26F8D5786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B0EFD9-57F8-491B-A3EA-6239EDB352DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="GMSL" sheetId="1" r:id="rId1"/>
     <sheet name="Steric" sheetId="2" r:id="rId2"/>
-    <sheet name="Glaciers" sheetId="3" r:id="rId3"/>
+    <sheet name="GIC" sheetId="3" r:id="rId3"/>
     <sheet name="GrIS" sheetId="5" r:id="rId4"/>
     <sheet name="AIS" sheetId="4" r:id="rId5"/>
     <sheet name="WAIS" sheetId="6" r:id="rId6"/>
     <sheet name="EAIS" sheetId="7" r:id="rId7"/>
     <sheet name="PEN" sheetId="9" r:id="rId8"/>
-    <sheet name="AllButGlaciers" sheetId="13" r:id="rId9"/>
+    <sheet name="All but GIC" sheetId="13" r:id="rId9"/>
     <sheet name="Expert" sheetId="8" r:id="rId10"/>
     <sheet name="transposed ar6" sheetId="11" r:id="rId11"/>
     <sheet name="Frederikse" sheetId="12" r:id="rId12"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="91">
   <si>
     <t>#</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>gmslsigma</t>
+  </si>
+  <si>
+    <t>#glac numbers from https://link.springer.com/article/10.1007/s10712-011-9121-7</t>
+  </si>
+  <si>
+    <t>1850-1900</t>
   </si>
 </sst>
 </file>
@@ -711,7 +717,7 @@
   <dimension ref="A1:R22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:K10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -947,7 +953,7 @@
     </row>
     <row r="10" spans="1:18" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>90</v>
       </c>
       <c r="B10" s="1">
         <v>1850</v>
@@ -1309,7 +1315,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4941,8 +4947,8 @@
   </sheetPr>
   <dimension ref="A1:T13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -5168,6 +5174,24 @@
       <c r="T9" s="16"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1850</v>
+      </c>
+      <c r="C10" s="5">
+        <v>1900</v>
+      </c>
+      <c r="E10">
+        <v>0.434</v>
+      </c>
+      <c r="F10">
+        <v>0.11</v>
+      </c>
+      <c r="G10" t="s">
+        <v>89</v>
+      </c>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
       <c r="P10" s="16"/>
@@ -6077,15 +6101,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0414F62-F26B-4AD1-AB30-17B83DAD40A3}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S10" sqref="S10:W10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -6102,7 +6126,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -6116,12 +6140,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -6146,20 +6170,20 @@
       <c r="H4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J4" t="s">
+      <c r="Q4" t="s">
         <v>87</v>
       </c>
-      <c r="K4" t="s">
+      <c r="R4" t="s">
         <v>88</v>
       </c>
-      <c r="L4" t="s">
+      <c r="S4" t="s">
         <v>85</v>
       </c>
-      <c r="M4" t="s">
+      <c r="T4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -6171,30 +6195,30 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5">
-        <f>J5-L5</f>
+        <f>Q5-S5</f>
         <v>0.77000000000000013</v>
       </c>
       <c r="F5">
-        <f>SQRT(K5^2+ M5^2)</f>
+        <f>SQRT(R5^2+ T5^2)</f>
         <v>0.37600136416247626</v>
       </c>
       <c r="G5" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="J5" s="21">
+      <c r="Q5" s="21">
         <v>1.35</v>
       </c>
-      <c r="K5" s="21">
+      <c r="R5" s="21">
         <v>0.34653615831230811</v>
       </c>
-      <c r="L5">
+      <c r="S5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="M5">
+      <c r="T5">
         <v>0.14590996139465603</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -6206,30 +6230,30 @@
       </c>
       <c r="D6" s="5"/>
       <c r="E6">
-        <f>J6-L6</f>
+        <f>Q6-S6</f>
         <v>1.8900000000000001</v>
       </c>
       <c r="F6">
-        <f>SQRT(K6^2+ M6^2)</f>
+        <f>SQRT(R6^2+ T6^2)</f>
         <v>0.49731015669922207</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="J6" s="21">
+      <c r="Q6" s="21">
         <v>2.33</v>
       </c>
-      <c r="K6" s="21">
+      <c r="R6" s="21">
         <v>0.47724716539502088</v>
       </c>
-      <c r="L6">
+      <c r="S6">
         <v>0.44</v>
       </c>
-      <c r="M6">
+      <c r="T6">
         <v>0.13983037966987874</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>44</v>
       </c>
@@ -6241,30 +6265,30 @@
       </c>
       <c r="D7" s="5"/>
       <c r="E7">
-        <f>J7-L7</f>
+        <f>Q7-S7</f>
         <v>2.7</v>
       </c>
       <c r="F7">
-        <f>SQRT(K7^2+ M7^2)</f>
+        <f>SQRT(R7^2+ T7^2)</f>
         <v>0.23991249685230437</v>
       </c>
       <c r="G7" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="16">
+      <c r="Q7" s="16">
         <v>3.25</v>
       </c>
-      <c r="K7" s="16">
+      <c r="R7" s="16">
         <v>0.22190473295437274</v>
       </c>
-      <c r="L7">
+      <c r="S7">
         <v>0.55000000000000004</v>
       </c>
-      <c r="M7">
+      <c r="T7">
         <v>9.1193725871660011E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>46</v>
       </c>
@@ -6276,30 +6300,30 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8">
-        <f>J8-L8</f>
+        <f>Q8-S8</f>
         <v>3.07</v>
       </c>
       <c r="F8">
-        <f>SQRT(K8^2+ M8^2)</f>
+        <f>SQRT(R8^2+ T8^2)</f>
         <v>0.29372937729089094</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="J8">
+      <c r="Q8">
         <v>3.69</v>
       </c>
-      <c r="K8">
+      <c r="R8">
         <v>0.29181992278931213</v>
       </c>
-      <c r="L8">
+      <c r="S8">
         <v>0.62</v>
       </c>
-      <c r="M8">
+      <c r="T8">
         <v>3.3437699486275375E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -6311,30 +6335,30 @@
       </c>
       <c r="D9" s="5"/>
       <c r="E9">
-        <f>J9-L9</f>
+        <f>Q9-S9</f>
         <v>1.1600000000000001</v>
       </c>
       <c r="F9">
-        <f>SQRT(K9^2+ M9^2)</f>
+        <f>SQRT(R9^2+ T9^2)</f>
         <v>0.30046299159562434</v>
       </c>
       <c r="G9" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="J9">
+      <c r="Q9">
         <v>1.73</v>
       </c>
-      <c r="K9">
+      <c r="R9">
         <v>0.27054138675259143</v>
       </c>
-      <c r="L9">
+      <c r="S9">
         <v>0.56999999999999995</v>
       </c>
-      <c r="M9">
+      <c r="T9">
         <v>0.13071100708271274</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
@@ -6346,12 +6370,12 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10">
-        <f>J10-L10</f>
-        <v>0.28000000000000003</v>
+        <f>Q10-S10</f>
+        <v>-0.15399999999999997</v>
       </c>
       <c r="F10">
-        <f>SQRT(K10^2+ M10^2)</f>
-        <v>0.28000000000000003</v>
+        <f>SQRT(R10^2+ T10^2)</f>
+        <v>0.30083217912982646</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>18</v>
@@ -6359,13 +6383,22 @@
       <c r="H10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="J10" s="5">
+      <c r="Q10" s="5">
         <f>0.014*1000/50</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="K10" s="5">
+      <c r="R10" s="5">
         <f>0.014*1000/50</f>
         <v>0.28000000000000003</v>
+      </c>
+      <c r="S10">
+        <v>0.434</v>
+      </c>
+      <c r="T10">
+        <v>0.11</v>
+      </c>
+      <c r="V10" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>